<commit_message>
adding table file file
</commit_message>
<xml_diff>
--- a/project/DatabaseTables (1).xlsx
+++ b/project/DatabaseTables (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalit kumar\Desktop\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vikash\Hospital-Management-Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25482A42-E3B3-4894-9F6A-AC06F84A86BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5738E631-AAC7-4BE4-AC58-424EFE35B08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{80D25240-4AFC-4227-AA70-7B489448DFE0}"/>
   </bookViews>
@@ -713,7 +713,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
@@ -751,6 +751,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1070,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBFBCCE-F544-4EFA-AD02-7BFEEFE2F45C}">
   <dimension ref="A2:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,11 +1681,11 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
         <v>44</v>
@@ -1697,13 +1700,13 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="33" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="6"/>
@@ -1717,13 +1720,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
         <v>129</v>
@@ -1742,13 +1745,13 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="6"/>
       <c r="F33" s="26" t="s">
         <v>109</v>
@@ -1769,13 +1772,13 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="6"/>
       <c r="F34" s="20"/>
       <c r="G34" s="6"/>
@@ -1792,13 +1795,13 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="36" t="s">
         <v>42</v>
       </c>
       <c r="E35" s="6"/>
@@ -1822,11 +1825,11 @@
       <c r="C37" s="20"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="39"/>
       <c r="J37" s="22" t="s">
         <v>76</v>
       </c>
@@ -1837,13 +1840,13 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G38" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="H38" s="7" t="s">
+      <c r="H38" s="33" t="s">
         <v>53</v>
       </c>
       <c r="J38" t="s">
@@ -1866,13 +1869,13 @@
       <c r="E39" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="H39" s="7"/>
+      <c r="H39" s="33"/>
       <c r="J39" t="s">
         <v>79</v>
       </c>
@@ -1895,13 +1898,13 @@
         <v>53</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H40" s="7"/>
+      <c r="H40" s="33"/>
       <c r="J40" t="s">
         <v>64</v>
       </c>
@@ -1922,13 +1925,13 @@
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="24" t="s">
+      <c r="F41" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="H41" s="7"/>
+      <c r="H41" s="33"/>
       <c r="J41" t="s">
         <v>46</v>
       </c>
@@ -1951,13 +1954,13 @@
         <v>65</v>
       </c>
       <c r="E42" s="6"/>
-      <c r="F42" s="26" t="s">
+      <c r="F42" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="H42" s="27" t="s">
+      <c r="H42" s="36" t="s">
         <v>42</v>
       </c>
       <c r="J42" t="s">

</xml_diff>